<commit_message>
New graph map implementation. Removed TribeMap. Refactored cell posisitioning system. Added log filtering
</commit_message>
<xml_diff>
--- a/docs/map_cell_position_example.xlsx
+++ b/docs/map_cell_position_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\ISU\Documents\git\WorldOfAgents\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F75E2CDE-FBC6-4202-B874-6026FE03E5E1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72A17D4-94CC-4054-9E94-4818DDD729F7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="2550" windowWidth="21600" windowHeight="11385" xr2:uid="{58829FEF-A7B3-4614-8629-B705DE25067C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{58829FEF-A7B3-4614-8629-B705DE25067C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="28">
   <si>
     <t>00</t>
   </si>
@@ -109,13 +109,19 @@
   </si>
   <si>
     <t>82</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>Map must be square and even sided to be able to fit into a hex grid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,8 +142,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,8 +182,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -177,11 +203,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -194,6 +300,24 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,18 +632,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E60B704A-59B7-41B3-A485-675DF78E5EDC}">
-  <dimension ref="B1:V21"/>
+  <dimension ref="B1:AM39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="V7" sqref="V7"/>
+    <sheetView tabSelected="1" topLeftCell="K6" workbookViewId="0">
+      <selection activeCell="AE31" sqref="AE31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:30" x14ac:dyDescent="0.25">
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:30" x14ac:dyDescent="0.25">
       <c r="E2" s="3"/>
       <c r="F2" s="9" t="s">
         <v>1</v>
@@ -549,7 +673,7 @@
       <c r="S2" s="3"/>
       <c r="T2" s="3"/>
     </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:30" x14ac:dyDescent="0.25">
       <c r="E3" s="10" t="s">
         <v>0</v>
       </c>
@@ -583,7 +707,7 @@
       </c>
       <c r="T3" s="3"/>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:30" x14ac:dyDescent="0.25">
       <c r="E4" s="3"/>
       <c r="F4" s="1">
         <v>11</v>
@@ -615,7 +739,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>20</v>
       </c>
@@ -655,7 +779,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:30" x14ac:dyDescent="0.25">
       <c r="E6" s="3"/>
       <c r="F6" s="1">
         <v>31</v>
@@ -687,7 +811,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:30" x14ac:dyDescent="0.25">
       <c r="E7" s="10" t="s">
         <v>18</v>
       </c>
@@ -721,7 +845,7 @@
       </c>
       <c r="T7" s="3"/>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:30" x14ac:dyDescent="0.25">
       <c r="E8" s="3"/>
       <c r="F8" s="1">
         <v>51</v>
@@ -752,8 +876,20 @@
       <c r="T8" s="11">
         <v>57</v>
       </c>
-    </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="Y8" s="1">
+        <v>11</v>
+      </c>
+      <c r="Z8" s="4"/>
+      <c r="AA8" s="1">
+        <v>13</v>
+      </c>
+      <c r="AB8" s="4"/>
+      <c r="AC8" s="6">
+        <v>15</v>
+      </c>
+      <c r="AD8" s="4"/>
+    </row>
+    <row r="9" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>13</v>
       </c>
@@ -766,7 +902,7 @@
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="10" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="10" t="s">
@@ -789,8 +925,20 @@
         <v>5</v>
       </c>
       <c r="T9" s="3"/>
-    </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="6">
+        <v>22</v>
+      </c>
+      <c r="AA9" s="4"/>
+      <c r="AB9" s="6">
+        <v>24</v>
+      </c>
+      <c r="AC9" s="4"/>
+      <c r="AD9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>14</v>
       </c>
@@ -822,14 +970,38 @@
       </c>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
-    </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="Y10" s="1">
+        <v>31</v>
+      </c>
+      <c r="Z10" s="4"/>
+      <c r="AA10" s="1">
+        <v>33</v>
+      </c>
+      <c r="AB10" s="4"/>
+      <c r="AC10" s="6">
+        <v>35</v>
+      </c>
+      <c r="AD10" s="4"/>
+    </row>
+    <row r="11" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
       <c r="L11" s="5"/>
-    </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="Y11" s="4"/>
+      <c r="Z11" s="1">
+        <v>42</v>
+      </c>
+      <c r="AA11" s="4"/>
+      <c r="AB11" s="6">
+        <v>44</v>
+      </c>
+      <c r="AC11" s="4"/>
+      <c r="AD11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="2:30" x14ac:dyDescent="0.25">
       <c r="E12" s="3"/>
       <c r="F12" s="9" t="s">
         <v>1</v>
@@ -856,8 +1028,20 @@
         <v>11</v>
       </c>
       <c r="S12" s="3"/>
-    </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="Y12" s="6">
+        <v>51</v>
+      </c>
+      <c r="Z12" s="4"/>
+      <c r="AA12" s="6">
+        <v>53</v>
+      </c>
+      <c r="AB12" s="4"/>
+      <c r="AC12" s="1">
+        <v>55</v>
+      </c>
+      <c r="AD12" s="4"/>
+    </row>
+    <row r="13" spans="2:30" x14ac:dyDescent="0.25">
       <c r="E13" s="10" t="s">
         <v>0</v>
       </c>
@@ -889,8 +1073,20 @@
         <v>12</v>
       </c>
       <c r="T13" s="3"/>
-    </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA13" s="4"/>
+      <c r="AB13">
+        <v>64</v>
+      </c>
+      <c r="AC13" s="4"/>
+      <c r="AD13" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:30" x14ac:dyDescent="0.25">
       <c r="E14" s="3"/>
       <c r="F14" s="1">
         <v>11</v>
@@ -921,7 +1117,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:30" x14ac:dyDescent="0.25">
       <c r="E15" s="10" t="s">
         <v>17</v>
       </c>
@@ -954,7 +1150,7 @@
       </c>
       <c r="T15" s="3"/>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>21</v>
       </c>
@@ -991,7 +1187,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="5:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:39" x14ac:dyDescent="0.25">
       <c r="E17" s="10" t="s">
         <v>18</v>
       </c>
@@ -1024,7 +1220,7 @@
       </c>
       <c r="T17" s="3"/>
     </row>
-    <row r="18" spans="5:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:39" x14ac:dyDescent="0.25">
       <c r="E18" s="3"/>
       <c r="F18" s="1">
         <v>51</v>
@@ -1055,7 +1251,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="5:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:39" x14ac:dyDescent="0.25">
       <c r="E19" s="10" t="s">
         <v>19</v>
       </c>
@@ -1079,8 +1275,8 @@
         <v>3</v>
       </c>
       <c r="P19" s="4"/>
-      <c r="Q19" t="s">
-        <v>5</v>
+      <c r="Q19">
+        <v>64</v>
       </c>
       <c r="R19" s="4"/>
       <c r="S19" t="s">
@@ -1088,7 +1284,7 @@
       </c>
       <c r="T19" s="3"/>
     </row>
-    <row r="20" spans="5:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:39" x14ac:dyDescent="0.25">
       <c r="E20" s="3"/>
       <c r="F20" s="11" t="s">
         <v>2</v>
@@ -1118,8 +1314,11 @@
       <c r="T20" s="11">
         <v>77</v>
       </c>
-    </row>
-    <row r="21" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="V20" s="29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="5:39" x14ac:dyDescent="0.25">
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="10" t="s">
@@ -1146,6 +1345,546 @@
       </c>
       <c r="T21" s="3"/>
     </row>
+    <row r="22" spans="5:39" x14ac:dyDescent="0.25">
+      <c r="V22" s="12">
+        <v>11</v>
+      </c>
+      <c r="W22" s="13"/>
+      <c r="X22" s="12">
+        <v>13</v>
+      </c>
+      <c r="Y22" s="13"/>
+      <c r="Z22" s="12">
+        <v>15</v>
+      </c>
+      <c r="AA22" s="13"/>
+      <c r="AB22" s="12">
+        <v>11</v>
+      </c>
+      <c r="AC22" s="13"/>
+      <c r="AD22" s="12">
+        <v>13</v>
+      </c>
+      <c r="AE22" s="13"/>
+      <c r="AF22" s="12">
+        <v>15</v>
+      </c>
+      <c r="AG22" s="13"/>
+    </row>
+    <row r="23" spans="5:39" x14ac:dyDescent="0.25">
+      <c r="V23" s="13"/>
+      <c r="W23" s="12">
+        <v>22</v>
+      </c>
+      <c r="X23" s="13"/>
+      <c r="Y23" s="12">
+        <v>24</v>
+      </c>
+      <c r="Z23" s="13"/>
+      <c r="AA23" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB23" s="13"/>
+      <c r="AC23" s="12">
+        <v>22</v>
+      </c>
+      <c r="AD23" s="13"/>
+      <c r="AE23" s="12">
+        <v>24</v>
+      </c>
+      <c r="AF23" s="13"/>
+      <c r="AG23" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="5:39" x14ac:dyDescent="0.25">
+      <c r="V24" s="12">
+        <v>31</v>
+      </c>
+      <c r="W24" s="13"/>
+      <c r="X24" s="12">
+        <v>33</v>
+      </c>
+      <c r="Y24" s="13"/>
+      <c r="Z24" s="12">
+        <v>35</v>
+      </c>
+      <c r="AA24" s="13"/>
+      <c r="AB24" s="12">
+        <v>31</v>
+      </c>
+      <c r="AC24" s="13"/>
+      <c r="AD24" s="12">
+        <v>33</v>
+      </c>
+      <c r="AE24" s="13"/>
+      <c r="AF24" s="12">
+        <v>35</v>
+      </c>
+      <c r="AG24" s="13"/>
+    </row>
+    <row r="25" spans="5:39" x14ac:dyDescent="0.25">
+      <c r="V25" s="13"/>
+      <c r="W25" s="12">
+        <v>42</v>
+      </c>
+      <c r="X25" s="13"/>
+      <c r="Y25" s="12">
+        <v>44</v>
+      </c>
+      <c r="Z25" s="13"/>
+      <c r="AA25" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB25" s="13"/>
+      <c r="AC25" s="12">
+        <v>42</v>
+      </c>
+      <c r="AD25" s="13"/>
+      <c r="AE25" s="12">
+        <v>44</v>
+      </c>
+      <c r="AF25" s="13"/>
+      <c r="AG25" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="5:39" x14ac:dyDescent="0.25">
+      <c r="V26" s="12">
+        <v>51</v>
+      </c>
+      <c r="W26" s="13"/>
+      <c r="X26" s="12">
+        <v>53</v>
+      </c>
+      <c r="Y26" s="13"/>
+      <c r="Z26" s="12">
+        <v>55</v>
+      </c>
+      <c r="AA26" s="13"/>
+      <c r="AB26" s="12">
+        <v>51</v>
+      </c>
+      <c r="AC26" s="13"/>
+      <c r="AD26" s="12">
+        <v>53</v>
+      </c>
+      <c r="AE26" s="13"/>
+      <c r="AF26" s="12">
+        <v>55</v>
+      </c>
+      <c r="AG26" s="13"/>
+    </row>
+    <row r="27" spans="5:39" x14ac:dyDescent="0.25">
+      <c r="V27" s="13"/>
+      <c r="W27" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="X27" s="13"/>
+      <c r="Y27" s="14">
+        <v>64</v>
+      </c>
+      <c r="Z27" s="13"/>
+      <c r="AA27" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB27" s="13"/>
+      <c r="AC27" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD27" s="13"/>
+      <c r="AE27" s="14">
+        <v>64</v>
+      </c>
+      <c r="AF27" s="13"/>
+      <c r="AG27" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="5:39" x14ac:dyDescent="0.25">
+      <c r="V28" s="12">
+        <v>11</v>
+      </c>
+      <c r="W28" s="13"/>
+      <c r="X28" s="12">
+        <v>13</v>
+      </c>
+      <c r="Y28" s="13"/>
+      <c r="Z28" s="12">
+        <v>15</v>
+      </c>
+      <c r="AA28" s="13"/>
+      <c r="AB28" s="1">
+        <v>11</v>
+      </c>
+      <c r="AC28" s="4"/>
+      <c r="AD28" s="1">
+        <v>13</v>
+      </c>
+      <c r="AE28" s="4"/>
+      <c r="AF28" s="1">
+        <v>15</v>
+      </c>
+      <c r="AG28" s="4"/>
+      <c r="AH28" s="12">
+        <v>11</v>
+      </c>
+      <c r="AI28" s="13"/>
+      <c r="AJ28" s="12">
+        <v>13</v>
+      </c>
+      <c r="AK28" s="13"/>
+      <c r="AL28" s="12">
+        <v>15</v>
+      </c>
+      <c r="AM28" s="13"/>
+    </row>
+    <row r="29" spans="5:39" x14ac:dyDescent="0.25">
+      <c r="V29" s="13"/>
+      <c r="W29" s="12">
+        <v>22</v>
+      </c>
+      <c r="X29" s="13"/>
+      <c r="Y29" s="12">
+        <v>24</v>
+      </c>
+      <c r="Z29" s="13"/>
+      <c r="AA29" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB29" s="4"/>
+      <c r="AC29" s="1">
+        <v>22</v>
+      </c>
+      <c r="AD29" s="4"/>
+      <c r="AE29" s="1">
+        <v>24</v>
+      </c>
+      <c r="AF29" s="4"/>
+      <c r="AG29" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH29" s="13"/>
+      <c r="AI29" s="12">
+        <v>22</v>
+      </c>
+      <c r="AJ29" s="13"/>
+      <c r="AK29" s="12">
+        <v>24</v>
+      </c>
+      <c r="AL29" s="13"/>
+      <c r="AM29" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="5:39" x14ac:dyDescent="0.25">
+      <c r="V30" s="12">
+        <v>31</v>
+      </c>
+      <c r="W30" s="13"/>
+      <c r="X30" s="12">
+        <v>33</v>
+      </c>
+      <c r="Y30" s="13"/>
+      <c r="Z30" s="12">
+        <v>35</v>
+      </c>
+      <c r="AA30" s="13"/>
+      <c r="AB30" s="1">
+        <v>31</v>
+      </c>
+      <c r="AC30" s="4"/>
+      <c r="AD30" s="1">
+        <v>33</v>
+      </c>
+      <c r="AE30" s="4"/>
+      <c r="AF30" s="1">
+        <v>35</v>
+      </c>
+      <c r="AG30" s="4"/>
+      <c r="AH30" s="12">
+        <v>31</v>
+      </c>
+      <c r="AI30" s="13"/>
+      <c r="AJ30" s="12">
+        <v>33</v>
+      </c>
+      <c r="AK30" s="13"/>
+      <c r="AL30" s="12">
+        <v>35</v>
+      </c>
+      <c r="AM30" s="13"/>
+    </row>
+    <row r="31" spans="5:39" x14ac:dyDescent="0.25">
+      <c r="V31" s="13"/>
+      <c r="W31" s="12">
+        <v>42</v>
+      </c>
+      <c r="X31" s="13"/>
+      <c r="Y31" s="12">
+        <v>44</v>
+      </c>
+      <c r="Z31" s="13"/>
+      <c r="AA31" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB31" s="4"/>
+      <c r="AC31" s="1">
+        <v>42</v>
+      </c>
+      <c r="AD31" s="4"/>
+      <c r="AE31" s="1">
+        <v>44</v>
+      </c>
+      <c r="AF31" s="15"/>
+      <c r="AG31" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH31" s="17"/>
+      <c r="AI31" s="12">
+        <v>42</v>
+      </c>
+      <c r="AJ31" s="13"/>
+      <c r="AK31" s="12">
+        <v>44</v>
+      </c>
+      <c r="AL31" s="13"/>
+      <c r="AM31" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="5:39" x14ac:dyDescent="0.25">
+      <c r="V32" s="12">
+        <v>51</v>
+      </c>
+      <c r="W32" s="13"/>
+      <c r="X32" s="12">
+        <v>53</v>
+      </c>
+      <c r="Y32" s="13"/>
+      <c r="Z32" s="12">
+        <v>55</v>
+      </c>
+      <c r="AA32" s="13"/>
+      <c r="AB32" s="1">
+        <v>51</v>
+      </c>
+      <c r="AC32" s="4"/>
+      <c r="AD32" s="1">
+        <v>53</v>
+      </c>
+      <c r="AE32" s="4"/>
+      <c r="AF32" s="18">
+        <v>55</v>
+      </c>
+      <c r="AG32" s="19"/>
+      <c r="AH32" s="20">
+        <v>51</v>
+      </c>
+      <c r="AI32" s="13"/>
+      <c r="AJ32" s="12">
+        <v>53</v>
+      </c>
+      <c r="AK32" s="13"/>
+      <c r="AL32" s="12">
+        <v>55</v>
+      </c>
+      <c r="AM32" s="13"/>
+    </row>
+    <row r="33" spans="22:39" x14ac:dyDescent="0.25">
+      <c r="V33" s="13"/>
+      <c r="W33" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="X33" s="13"/>
+      <c r="Y33" s="14">
+        <v>64</v>
+      </c>
+      <c r="Z33" s="13"/>
+      <c r="AA33" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB33" s="4"/>
+      <c r="AC33">
+        <v>62</v>
+      </c>
+      <c r="AD33" s="4"/>
+      <c r="AE33">
+        <v>64</v>
+      </c>
+      <c r="AF33" s="21"/>
+      <c r="AG33" s="22">
+        <v>66</v>
+      </c>
+      <c r="AH33" s="23"/>
+      <c r="AI33" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ33" s="13"/>
+      <c r="AK33" s="14">
+        <v>64</v>
+      </c>
+      <c r="AL33" s="13"/>
+      <c r="AM33" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="22:39" x14ac:dyDescent="0.25">
+      <c r="AB34" s="12">
+        <v>11</v>
+      </c>
+      <c r="AC34" s="13"/>
+      <c r="AD34" s="12">
+        <v>13</v>
+      </c>
+      <c r="AE34" s="13"/>
+      <c r="AF34" s="24">
+        <v>15</v>
+      </c>
+      <c r="AG34" s="25"/>
+      <c r="AH34" s="20">
+        <v>11</v>
+      </c>
+      <c r="AI34" s="13"/>
+      <c r="AJ34" s="12">
+        <v>13</v>
+      </c>
+      <c r="AK34" s="13"/>
+      <c r="AL34" s="12">
+        <v>15</v>
+      </c>
+      <c r="AM34" s="13"/>
+    </row>
+    <row r="35" spans="22:39" x14ac:dyDescent="0.25">
+      <c r="AB35" s="13"/>
+      <c r="AC35" s="12">
+        <v>22</v>
+      </c>
+      <c r="AD35" s="13"/>
+      <c r="AE35" s="12">
+        <v>24</v>
+      </c>
+      <c r="AF35" s="26"/>
+      <c r="AG35" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH35" s="28"/>
+      <c r="AI35" s="12">
+        <v>22</v>
+      </c>
+      <c r="AJ35" s="13"/>
+      <c r="AK35" s="12">
+        <v>24</v>
+      </c>
+      <c r="AL35" s="13"/>
+      <c r="AM35" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="22:39" x14ac:dyDescent="0.25">
+      <c r="AB36" s="12">
+        <v>31</v>
+      </c>
+      <c r="AC36" s="13"/>
+      <c r="AD36" s="12">
+        <v>33</v>
+      </c>
+      <c r="AE36" s="13"/>
+      <c r="AF36" s="12">
+        <v>35</v>
+      </c>
+      <c r="AG36" s="13"/>
+      <c r="AH36" s="12">
+        <v>31</v>
+      </c>
+      <c r="AI36" s="13"/>
+      <c r="AJ36" s="12">
+        <v>33</v>
+      </c>
+      <c r="AK36" s="13"/>
+      <c r="AL36" s="12">
+        <v>35</v>
+      </c>
+      <c r="AM36" s="13"/>
+    </row>
+    <row r="37" spans="22:39" x14ac:dyDescent="0.25">
+      <c r="AB37" s="13"/>
+      <c r="AC37" s="12">
+        <v>42</v>
+      </c>
+      <c r="AD37" s="13"/>
+      <c r="AE37" s="12">
+        <v>44</v>
+      </c>
+      <c r="AF37" s="13"/>
+      <c r="AG37" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH37" s="13"/>
+      <c r="AI37" s="12">
+        <v>42</v>
+      </c>
+      <c r="AJ37" s="13"/>
+      <c r="AK37" s="12">
+        <v>44</v>
+      </c>
+      <c r="AL37" s="13"/>
+      <c r="AM37" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="22:39" x14ac:dyDescent="0.25">
+      <c r="AB38" s="12">
+        <v>51</v>
+      </c>
+      <c r="AC38" s="13"/>
+      <c r="AD38" s="12">
+        <v>53</v>
+      </c>
+      <c r="AE38" s="13"/>
+      <c r="AF38" s="12">
+        <v>55</v>
+      </c>
+      <c r="AG38" s="13"/>
+      <c r="AH38" s="12">
+        <v>51</v>
+      </c>
+      <c r="AI38" s="13"/>
+      <c r="AJ38" s="12">
+        <v>53</v>
+      </c>
+      <c r="AK38" s="13"/>
+      <c r="AL38" s="12">
+        <v>55</v>
+      </c>
+      <c r="AM38" s="13"/>
+    </row>
+    <row r="39" spans="22:39" x14ac:dyDescent="0.25">
+      <c r="AB39" s="13"/>
+      <c r="AC39" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD39" s="13"/>
+      <c r="AE39" s="14">
+        <v>64</v>
+      </c>
+      <c r="AF39" s="13"/>
+      <c r="AG39" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH39" s="13"/>
+      <c r="AI39" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ39" s="13"/>
+      <c r="AK39" s="14">
+        <v>64</v>
+      </c>
+      <c r="AL39" s="13"/>
+      <c r="AM39" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>